<commit_message>
Added the New test cases
Signed-off-by: Jabesh <starjabesh@gmail.com>
</commit_message>
<xml_diff>
--- a/src/main/resources/com/orangehrm/data/TestData.xlsx
+++ b/src/main/resources/com/orangehrm/data/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -48,14 +48,20 @@
     <t>2021-Apr-23</t>
   </si>
   <si>
-    <t>Paul Collings</t>
+    <t>Mily Hm</t>
+  </si>
+  <si>
+    <t>testcase2</t>
+  </si>
+  <si>
+    <t>jabesh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -138,12 +144,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -190,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,9 +239,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,6 +274,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -431,19 +450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="F3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.6640625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -463,7 +482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -480,6 +499,26 @@
         <v>9</v>
       </c>
       <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
     </row>
@@ -490,24 +529,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>